<commit_message>
Added RT Engine to project
</commit_message>
<xml_diff>
--- a/VI/HMI/Data/Template Excel/X1111.xlsx
+++ b/VI/HMI/Data/Template Excel/X1111.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SNG_THINKPAD\Documents\g159-one-subsea-test-pressure-monitoring-system\VI\HMI\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasni\Desktop\OSS V1\HMI\Data\Template Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D0DD00C-AB69-4416-BC2D-F25AA6A490C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597203D4-C5BE-4C72-938F-B1659EEB7025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F2F939B5-6682-448B-9C73-AC87332BC915}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F2F939B5-6682-448B-9C73-AC87332BC915}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -875,7 +875,7 @@
   <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,7 +990,7 @@
         <v>24</v>
       </c>
       <c r="M2" s="43">
-        <v>15000</v>
+        <v>4000</v>
       </c>
       <c r="N2" s="41" t="s">
         <v>25</v>
@@ -1035,7 +1035,7 @@
         <v>24</v>
       </c>
       <c r="M3" s="43">
-        <v>15000</v>
+        <v>4000</v>
       </c>
       <c r="N3" s="41" t="s">
         <v>27</v>
@@ -1995,7 +1995,7 @@
       <c r="R24" s="24"/>
       <c r="S24" s="25"/>
     </row>
-    <row r="25" spans="1:19" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="35"/>
       <c r="B25" s="35"/>
       <c r="C25" s="35"/>

</xml_diff>